<commit_message>
Scripts updated, computer generated data uploaded
</commit_message>
<xml_diff>
--- a/Parameters/Par_HUN_Reconstruction.xlsx
+++ b/Parameters/Par_HUN_Reconstruction.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Uncertainty" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="WaningPulse" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -60,33 +59,18 @@
     <t xml:space="preserve">Pr_D</t>
   </si>
   <si>
-    <t xml:space="preserve">Rel_omega</t>
-  </si>
-  <si>
     <t xml:space="preserve">New_Cases_Shift</t>
   </si>
   <si>
     <t xml:space="preserve">New_Cases_Mtp</t>
   </si>
   <si>
-    <t xml:space="preserve">Szennyviz_Shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Szennyviz_Mtp</t>
-  </si>
-  <si>
     <t xml:space="preserve">beta0</t>
   </si>
   <si>
     <t xml:space="preserve">beta_max</t>
   </si>
   <si>
-    <t xml:space="preserve">wnom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wmax</t>
-  </si>
-  <si>
     <t xml:space="preserve">Transient</t>
   </si>
   <si>
@@ -108,34 +92,13 @@
     <t xml:space="preserve">OmicronBA5</t>
   </si>
   <si>
-    <t xml:space="preserve">TurnPoint1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TurnPoint2</t>
+    <t xml:space="preserve">OmicronBA5_Tp1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OmicronBQ1</t>
   </si>
   <si>
     <t xml:space="preserve">Future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PulseDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PulseWidth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Immune evasion before the delta wave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omicron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Immune evasion before the omicron wave</t>
   </si>
 </sst>
 </file>
@@ -255,7 +218,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,7 +235,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,18 +276,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -406,23 +357,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="1" width="16.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="18" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="22" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="16.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1019" min="17" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,26 +425,11 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>43739</v>
@@ -529,37 +465,22 @@
         <v>0.205</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0.2</v>
+        <v>12</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>12</v>
+        <v>3.5</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>3.5</v>
+        <v>0.33</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="S2" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="T2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1"/>
+      <c r="Q2" s="1"/>
     </row>
     <row r="3" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>43936</v>
@@ -595,37 +516,27 @@
         <v>0.205</v>
       </c>
       <c r="M3" s="8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N3" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="O3" s="11" t="n">
+      <c r="N3" s="11" t="n">
         <v>3.5</v>
       </c>
-      <c r="P3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="R3" s="8" t="n">
+      <c r="O3" s="8" t="n">
         <v>0.33</v>
       </c>
-      <c r="S3" s="8" t="n">
+      <c r="P3" s="8" t="n">
         <v>0.5</v>
       </c>
-      <c r="T3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="U3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>44228</v>
@@ -661,37 +572,27 @@
         <v>0.26</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N4" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="O4" s="11" t="n">
+      <c r="N4" s="11" t="n">
         <v>3.6</v>
       </c>
-      <c r="P4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="11" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="R4" s="8" t="n">
+      <c r="O4" s="8" t="n">
         <v>0.5</v>
       </c>
-      <c r="S4" s="8" t="n">
+      <c r="P4" s="8" t="n">
         <v>0.6</v>
       </c>
-      <c r="T4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="U4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="V4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>44409</v>
@@ -727,37 +628,27 @@
         <v>0.24</v>
       </c>
       <c r="M5" s="8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="N5" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="O5" s="11" t="n">
+      <c r="N5" s="11" t="n">
         <v>4.5</v>
       </c>
-      <c r="P5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R5" s="8" t="n">
+      <c r="O5" s="8" t="n">
         <v>0.83</v>
       </c>
-      <c r="S5" s="8" t="n">
+      <c r="P5" s="8" t="n">
         <v>0.9</v>
       </c>
-      <c r="T5" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="U5" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="V5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>44562</v>
@@ -793,37 +684,27 @@
         <v>0.18</v>
       </c>
       <c r="M6" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N6" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="O6" s="11" t="n">
+      <c r="N6" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="P6" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R6" s="8" t="n">
+      <c r="O6" s="8" t="n">
         <v>1.7</v>
       </c>
-      <c r="S6" s="8" t="n">
+      <c r="P6" s="8" t="n">
         <v>1.8</v>
       </c>
-      <c r="T6" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="U6" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="V6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="AMF6" s="0"/>
+      <c r="AMG6" s="0"/>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>44621</v>
@@ -859,37 +740,27 @@
         <v>0.15</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N7" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="O7" s="11" t="n">
+      <c r="N7" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="P7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R7" s="8" t="n">
+      <c r="O7" s="8" t="n">
         <v>1.7</v>
       </c>
-      <c r="S7" s="8" t="n">
+      <c r="P7" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="T7" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="U7" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="V7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="AMF7" s="0"/>
+      <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>44727</v>
@@ -925,37 +796,27 @@
         <v>0.15</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N8" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="O8" s="11" t="n">
+      <c r="N8" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="P8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R8" s="8" t="n">
+      <c r="O8" s="8" t="n">
         <v>1.7</v>
       </c>
-      <c r="S8" s="8" t="n">
+      <c r="P8" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="T8" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="U8" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="V8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="AMF8" s="0"/>
+      <c r="AMG8" s="0"/>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>44804</v>
@@ -991,37 +852,27 @@
         <v>0.15</v>
       </c>
       <c r="M9" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="O9" s="11" t="n">
+      <c r="N9" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="P9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R9" s="8" t="n">
+      <c r="O9" s="8" t="n">
         <v>1.7</v>
       </c>
-      <c r="S9" s="8" t="n">
+      <c r="P9" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="T9" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="U9" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="V9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="AMF9" s="0"/>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>44883</v>
@@ -1057,37 +908,27 @@
         <v>0.15</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N10" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="11" t="n">
+      <c r="N10" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="P10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="11" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R10" s="8" t="n">
+      <c r="O10" s="8" t="n">
         <v>1.7</v>
       </c>
-      <c r="S10" s="8" t="n">
+      <c r="P10" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="T10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="U10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="V10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="AMF10" s="0"/>
+      <c r="AMG10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13" t="n">
         <v>45291</v>
@@ -1123,33 +964,18 @@
         <v>0.1</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>14</v>
+        <v>1.7</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R11" s="1" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="S11" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="T11" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="U11" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="V11" s="1"/>
+      <c r="Q11" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1169,11 +995,11 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -1240,98 +1066,6 @@
       </c>
       <c r="I2" s="14" t="n">
         <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="36.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="17" t="n">
-        <v>44402</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="D2" s="14" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="17" t="n">
-        <v>44558</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="D3" s="14" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>